<commit_message>
fixed date integration (aggregation) and dtype normalization
</commit_message>
<xml_diff>
--- a/references/Dominicks Financials from 1997 10-K.xlsx
+++ b/references/Dominicks Financials from 1997 10-K.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\mercor-dominicks-valuation\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\valuation\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6670DCB-2D20-4C70-827A-2A5EA15C6C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A4E2D-95C9-41DA-A9F6-31A8659F43C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51195" yWindow="0" windowWidth="25605" windowHeight="21600" activeTab="2" xr2:uid="{8E368467-3465-41D5-B8AE-57A786CB465E}"/>
+    <workbookView xWindow="41520" yWindow="1320" windowWidth="25590" windowHeight="21600" activeTab="1" xr2:uid="{8E368467-3465-41D5-B8AE-57A786CB465E}"/>
   </bookViews>
   <sheets>
     <sheet name="Extracted" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
   <si>
     <t xml:space="preserve"> Valuation Driver                </t>
   </si>
@@ -71,9 +71,6 @@
     <t>Page</t>
   </si>
   <si>
-    <t>Gross Margin</t>
-  </si>
-  <si>
     <t>Gross Profit</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>rounding_rule</t>
   </si>
   <si>
-    <t>gross_margin</t>
-  </si>
-  <si>
     <t>cogs_growth</t>
   </si>
   <si>
@@ -339,6 +333,21 @@
   </si>
   <si>
     <t>working_capital_deficit</t>
+  </si>
+  <si>
+    <t>Gross Margin Percentage</t>
+  </si>
+  <si>
+    <t>gross_margin_pct</t>
+  </si>
+  <si>
+    <t>Inventory Turnover</t>
+  </si>
+  <si>
+    <t>inventory_turnover</t>
+  </si>
+  <si>
+    <t>COGS/Inventory</t>
   </si>
 </sst>
 </file>
@@ -348,7 +357,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -402,7 +411,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -740,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -752,47 +761,47 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1">
         <v>2511962</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1">
         <v>1474982</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,167 +809,167 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1">
         <v>1932994</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1">
         <v>1136600</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1">
         <v>578968</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1">
         <v>491359</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1">
         <v>49588</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="1">
         <v>45924</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1">
         <v>203411</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1">
         <v>187787</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2">
         <v>9.1999999999999998E-2</v>
@@ -972,27 +981,27 @@
         <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1">
         <v>33700</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170FCFF9-6D6C-4921-9BA4-1B2F6E8FF609}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,178 +1035,193 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2">
         <f>(Sales-COGS)/Sales</f>
         <v>0.23048437834648772</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2">
         <f>SG_A/Sales</f>
         <v>0.19560765648524939</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="4">
         <f>C2-C3</f>
         <v>3.487672186123833E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" s="2">
         <f>Capital_Expenditures__CAPX/Sales</f>
         <v>1.9740744485784417E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2">
         <f>Depreciation___Amortization/Sales</f>
         <v>1.8282123694546334E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3">
         <f>365*Inventory/COGS</f>
         <v>38.409335466121469</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3">
         <f>365*Accounts_Payable/COGS</f>
         <v>35.459114203148069</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1">
         <f>Sales-Sales__Prior_Year</f>
         <v>1036980</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1">
         <f>COGS-COGS__Prior_Year</f>
         <v>796394</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1">
         <f>(DIO-DPO)/365*COGS_Growth</f>
         <v>6437.0918150806529</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1">
         <f>C11/(Sales_Growth*0.01)</f>
         <v>0.62075370933679075</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3">
+        <f>COGS/Inventory</f>
+        <v>9.5028980733588639</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF6029F-4EA5-4FA5-B8A8-542057E27CA5}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1223,86 +1247,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3">
         <v>0.15</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3">
         <v>0.35</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
         <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6">
         <v>1000</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
company and financials test
</commit_message>
<xml_diff>
--- a/references/Dominicks Financials from 1997 10-K.xlsx
+++ b/references/Dominicks Financials from 1997 10-K.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\valuation\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545200C6-29EB-415A-A158-2667B568E83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4713C82-594D-488D-8260-ACCE35ADCDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51195" yWindow="0" windowWidth="25605" windowHeight="21600" activeTab="1" xr2:uid="{8E368467-3465-41D5-B8AE-57A786CB465E}"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="25605" windowHeight="21600" xr2:uid="{8E368467-3465-41D5-B8AE-57A786CB465E}"/>
   </bookViews>
   <sheets>
     <sheet name="Extracted" sheetId="1" r:id="rId1"/>
@@ -18,43 +18,48 @@
     <sheet name="Benchmarks" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Accounts_Payable">Extracted!$C$11</definedName>
-    <definedName name="accounts_receivable">Extracted!$C$12</definedName>
-    <definedName name="average_total_assets">Extracted!$C$22</definedName>
-    <definedName name="Capital_Expenditures__CAPX">Extracted!$C$8</definedName>
+    <definedName name="Accounts_Payable">Extracted!$C$13</definedName>
+    <definedName name="accounts_receivable">Extracted!$C$14</definedName>
+    <definedName name="average_total_assets">Extracted!$C$25</definedName>
+    <definedName name="Capital_Expenditures__CAPX">Extracted!$C$10</definedName>
     <definedName name="COGS">Extracted!$C$4</definedName>
     <definedName name="COGS__Prior_Year">Extracted!$C$5</definedName>
-    <definedName name="COGS_Growth">Derived!$C$13</definedName>
-    <definedName name="current_assets">Extracted!$C$16</definedName>
-    <definedName name="current_assets_prior">Extracted!$C$18</definedName>
-    <definedName name="current_liabilities">Extracted!$C$17</definedName>
-    <definedName name="current_liabilities_prior">Extracted!$C$19</definedName>
-    <definedName name="Depreciation___Amortization">Extracted!$C$9</definedName>
-    <definedName name="DIO">Derived!$C$9</definedName>
-    <definedName name="DPO">Derived!$C$10</definedName>
-    <definedName name="ebit">Derived!$C$25</definedName>
-    <definedName name="ebitda">Extracted!$C$23</definedName>
-    <definedName name="Effective_Interest_Rate">Extracted!$C$13</definedName>
-    <definedName name="Gross_Profit">Extracted!$C$6</definedName>
+    <definedName name="COGS_Growth">Derived!$C$15</definedName>
+    <definedName name="cogs_growth_rate">Derived!$C$15</definedName>
+    <definedName name="current_assets">Extracted!$C$19</definedName>
+    <definedName name="current_assets_prior">Extracted!$C$21</definedName>
+    <definedName name="current_liabilities">Extracted!$C$20</definedName>
+    <definedName name="current_liabilities_prior">Extracted!$C$22</definedName>
+    <definedName name="Depreciation___Amortization">Extracted!$C$11</definedName>
+    <definedName name="DIO">Derived!$C$10</definedName>
+    <definedName name="DPO">Derived!$C$11</definedName>
+    <definedName name="ebit">Derived!$C$27</definedName>
+    <definedName name="ebitda">Extracted!$C$26</definedName>
+    <definedName name="Effective_Interest_Rate">Extracted!$C$15</definedName>
+    <definedName name="gross_profit">Extracted!$C$6</definedName>
     <definedName name="gross_profit_margin">Derived!$B$4</definedName>
-    <definedName name="Inventory">Extracted!$C$10</definedName>
-    <definedName name="invested_capital">Derived!$C$23</definedName>
-    <definedName name="net_income">Extracted!$C$15</definedName>
-    <definedName name="nwc_change">Derived!$C$14</definedName>
-    <definedName name="operating_income">Extracted!$C$14</definedName>
+    <definedName name="gross_profit_prior">Extracted!$C$7</definedName>
+    <definedName name="Inventory">Extracted!$C$12</definedName>
+    <definedName name="invested_capital">Derived!$C$25</definedName>
+    <definedName name="net_income">Extracted!$C$18</definedName>
+    <definedName name="nwc_change">Derived!$C$16</definedName>
+    <definedName name="operating_income">Extracted!$C$16</definedName>
+    <definedName name="operating_income_prior">Extracted!$C$17</definedName>
     <definedName name="Rent_Expense">Extracted!#REF!</definedName>
     <definedName name="Sales">Extracted!$C$2</definedName>
     <definedName name="Sales__Prior_Year">Extracted!$C$3</definedName>
-    <definedName name="sales_growth">Derived!$C$11</definedName>
-    <definedName name="sales_growth_rate">Derived!$C$12</definedName>
-    <definedName name="SalesChange">Extracted!$C$14</definedName>
-    <definedName name="SG_A">Extracted!$C$7</definedName>
+    <definedName name="sales_growth">Derived!$C$12</definedName>
+    <definedName name="sales_growth_rate">Derived!$C$13</definedName>
+    <definedName name="SalesChange">Extracted!$C$17</definedName>
+    <definedName name="SG_A">Extracted!$C$9</definedName>
+    <definedName name="sga">Extracted!$C$8</definedName>
+    <definedName name="sga_prior">Extracted!$C$9</definedName>
     <definedName name="Store_Count">Extracted!#REF!</definedName>
     <definedName name="tax_rate">Benchmarks!$C$3</definedName>
-    <definedName name="total_debt">Extracted!$C$21</definedName>
-    <definedName name="total_shareholders_equity">Extracted!$C$20</definedName>
-    <definedName name="working_capital">Derived!$C$17</definedName>
-    <definedName name="working_capital_prior">Derived!$C$18</definedName>
+    <definedName name="total_debt">Extracted!$C$24</definedName>
+    <definedName name="total_shareholders_equity">Extracted!$C$23</definedName>
+    <definedName name="working_capital">Derived!$C$19</definedName>
+    <definedName name="working_capital_prior">Derived!$C$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="177">
   <si>
     <t xml:space="preserve"> Valuation Driver                </t>
   </si>
@@ -215,9 +220,6 @@
     <t>COGS (Prior Year)</t>
   </si>
   <si>
-    <t>COGS Growth</t>
-  </si>
-  <si>
     <t>∆NWC/(Sales Growth*0.01)</t>
   </si>
   <si>
@@ -546,6 +548,60 @@
   </si>
   <si>
     <t>(Current-Assets-Inventory) / Current Liabilities</t>
+  </si>
+  <si>
+    <t>COGS Growth Rate</t>
+  </si>
+  <si>
+    <t>cogs_growth_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COGS Growth </t>
+  </si>
+  <si>
+    <t>SG&amp;A (Prior Year)</t>
+  </si>
+  <si>
+    <t>sga_prior</t>
+  </si>
+  <si>
+    <t>SG&amp;A Growth</t>
+  </si>
+  <si>
+    <t>sga_growth</t>
+  </si>
+  <si>
+    <t>SG&amp;A - SG&amp;A (Prior Year)</t>
+  </si>
+  <si>
+    <t>Gross Profit (Prior Year)</t>
+  </si>
+  <si>
+    <t>gross_profit_prior</t>
+  </si>
+  <si>
+    <t>Gross Profit Growth</t>
+  </si>
+  <si>
+    <t>gross_profit_growth</t>
+  </si>
+  <si>
+    <t>Gross Profit - Gross Profit (Prior Year)</t>
+  </si>
+  <si>
+    <t>Operating Income Growth</t>
+  </si>
+  <si>
+    <t>operating_income_growth</t>
+  </si>
+  <si>
+    <t>Operating Income - Operating Income (Prior Year)</t>
+  </si>
+  <si>
+    <t>Operating Income (Prior Year)</t>
+  </si>
+  <si>
+    <t>operating_income_prior</t>
   </si>
 </sst>
 </file>
@@ -929,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D927DFAA-DD23-40D3-9BBA-8F1F4A946AE1}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -964,7 +1020,7 @@
         <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -972,7 +1028,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1">
         <v>2511962</v>
@@ -987,7 +1043,7 @@
         <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,7 +1051,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1">
         <f>1474982+958742</f>
@@ -1016,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1">
         <v>1932994</v>
@@ -1031,7 +1087,7 @@
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,7 +1095,7 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1">
         <f>1136600+747561</f>
@@ -1060,7 +1116,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1">
         <v>578968</v>
@@ -1075,18 +1131,19 @@
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1">
-        <v>491359</v>
+        <f>338382+211181</f>
+        <v>549563</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1095,243 +1152,260 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1">
-        <v>49588</v>
+        <v>491359</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="C9" s="1">
-        <v>45924</v>
+        <f>211181+293872</f>
+        <v>505053</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1">
-        <v>203411</v>
+        <v>49588</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1">
-        <v>187787</v>
+        <v>45924</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1">
-        <v>16723</v>
+        <v>203411</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
       </c>
       <c r="E12">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="1">
+        <v>187787</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16723</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>56</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="1">
-        <v>77109</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-6932</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1">
-        <v>274729</v>
+        <v>77109</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="C17" s="1">
-        <v>308434</v>
+        <f>44510-6970</f>
+        <v>37540</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1">
-        <v>274318</v>
+        <v>-6932</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1">
-        <v>308504</v>
+        <v>274729</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="E19">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1">
-        <v>1102205</v>
+        <v>308434</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1340,55 +1414,106 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1">
+        <v>274318</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="1">
+        <v>308504</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1102205</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C24" s="1">
+        <v>599400</v>
+      </c>
+      <c r="D24" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="1">
-        <v>599400</v>
-      </c>
-      <c r="D21" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21">
+      <c r="E24">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="C25" s="1">
         <f>(1102200+1100100)/2</f>
         <v>1101150</v>
       </c>
-      <c r="D22" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22">
+      <c r="D25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="C26" s="1">
         <v>134900</v>
       </c>
-      <c r="D23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23">
+      <c r="D26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26">
         <v>18</v>
       </c>
     </row>
@@ -1400,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170FCFF9-6D6C-4921-9BA4-1B2F6E8FF609}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1430,40 +1555,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
       </c>
       <c r="C2" s="2">
         <f>operating_income / Sales</f>
         <v>3.0696722323028773E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
       </c>
       <c r="C3" s="2">
         <f>net_income / Sales</f>
         <v>-2.7595958856065496E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
         <v>155</v>
-      </c>
-      <c r="B4" t="s">
-        <v>156</v>
       </c>
       <c r="C4" s="2">
         <f>(Sales-COGS)/Sales</f>
@@ -1478,11 +1603,11 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2">
         <f>SG_A/Sales</f>
-        <v>0.19560765648524939</v>
+        <v>0.20105917207346288</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -1490,314 +1615,374 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="1">
+        <f>sga-sga_prior</f>
+        <v>-13694</v>
+      </c>
+      <c r="D6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="4">
         <f>ebit/Sales</f>
         <v>3.5420917991593824E-2</v>
       </c>
-      <c r="D6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="2">
         <f>Capital_Expenditures__CAPX/Sales</f>
         <v>1.9740744485784417E-2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2">
         <f>Depreciation___Amortization/Sales</f>
         <v>1.8282123694546334E-2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3">
         <f>365*Inventory/COGS</f>
         <v>38.409335466121469</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="3">
         <f>365*Accounts_Payable/COGS</f>
         <v>35.459114203148069</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="1">
         <f>Sales-Sales__Prior_Year</f>
         <v>78238</v>
       </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="2">
         <f>(Sales-Sales__Prior_Year)/Sales</f>
         <v>3.1146171797184829E-2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="1">
+        <f>COGS-COGS__Prior_Year</f>
+        <v>48833</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="2">
         <f>(COGS-COGS__Prior_Year)/COGS__Prior_Year</f>
         <v>2.5917636550167423E-2</v>
       </c>
-      <c r="D13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1">
         <f>working_capital-working_capital_prior</f>
         <v>481</v>
       </c>
-      <c r="D14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1">
         <f>nwc_change/(sales_growth*0.01)</f>
         <v>0.61479076663513899</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
         <v>87</v>
       </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="C18" s="3">
         <f>COGS/Inventory</f>
         <v>9.5028980733588639</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
         <v>112</v>
       </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="C19" s="1">
         <f>current_assets-current_liabilities</f>
         <v>-33705</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D19" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B20" t="s">
         <v>115</v>
       </c>
-      <c r="B18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="C20" s="1">
         <f>current_assets_prior-current_liabilities_prior</f>
         <v>-34186</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
         <v>119</v>
       </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="C21" s="1">
         <f>current_assets / current_liabilities</f>
         <v>0.8907221642231401</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B22" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="C22" s="3">
         <f>total_debt / total_shareholders_equity</f>
         <v>0.54381898104254656</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B23" t="s">
         <v>130</v>
       </c>
-      <c r="B21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="C23" s="7">
         <f>net_income / average_total_assets</f>
         <v>-6.2952367978931119E-3</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D23" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="7">
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="7">
         <f>net_income / total_shareholders_equity</f>
         <v>-6.2892111721503715E-3</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="D24" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
         <v>140</v>
       </c>
-      <c r="B23" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="C25" s="1">
         <f>total_debt +total_shareholders_equity</f>
         <v>1701605</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D25" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="B26" t="s">
         <v>143</v>
       </c>
-      <c r="B24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="C26" s="2">
         <f>(ebit*(1-tax_rate))/invested_capital</f>
         <v>3.3988146485230124E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" t="s">
         <v>145</v>
       </c>
-      <c r="B25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="C27" s="1">
         <f>ebitda-(Depreciation___Amortization)</f>
         <v>88976</v>
       </c>
-      <c r="D25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
         <v>157</v>
       </c>
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="C28" s="1">
         <f>(current_assets-Inventory)/current_liabilities</f>
         <v>0.23122612941504503</v>
       </c>
-      <c r="D26" t="s">
-        <v>159</v>
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="1">
+        <f>gross_profit-gross_profit_prior</f>
+        <v>29405</v>
+      </c>
+      <c r="D29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="1">
+        <f>operating_income-operating_income_prior</f>
+        <v>39569</v>
+      </c>
+      <c r="D30" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1823,10 +2008,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1837,52 +2022,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3">
         <v>0.15</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3">
         <v>0.35</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
@@ -1893,16 +2078,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6">
         <v>1000</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>